<commit_message>
added rest of team to bible
</commit_message>
<xml_diff>
--- a/JumpingJax_bible.xlsx
+++ b/JumpingJax_bible.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\JJ-Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ambid\Documents\Coding\JJ-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92055845-CBC7-4CB1-AE3B-421457F8F97A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C04D1CA-9E88-473A-A818-CE8F870A4620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32895" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>Kevin Nilsson</t>
+  </si>
+  <si>
+    <t>Max "Hoots" Hooton</t>
+  </si>
+  <si>
+    <t>Zech Birkel</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Shane "Vhespir"</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -499,7 +514,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -633,18 +648,30 @@
       </c>
     </row>
     <row r="14" spans="4:6">
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="4:6">
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="4:6">
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="4:6">
@@ -740,7 +767,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="8">
         <f>COUNTIF(D2:D33,"*")</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added names we forgot
</commit_message>
<xml_diff>
--- a/JumpingJax_bible.xlsx
+++ b/JumpingJax_bible.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\JJ-Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ambid\Documents\Coding\JJ-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0171D19A-1BC7-4CA4-8F5C-A0E5C246F1B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAA5805-F372-433B-ACD5-551148EF7CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Sabien Jarmin</t>
-  </si>
-  <si>
     <t>Game director, lead Unity developer, level designer</t>
   </si>
   <si>
@@ -124,6 +121,33 @@
   </si>
   <si>
     <t>QA tester</t>
+  </si>
+  <si>
+    <t>Shane "Vhespir"</t>
+  </si>
+  <si>
+    <t>Composer</t>
+  </si>
+  <si>
+    <t>Logan "Ryver" Fairbairn</t>
+  </si>
+  <si>
+    <t>Character artist</t>
+  </si>
+  <si>
+    <t>Sabien "ambid" Jarmin</t>
+  </si>
+  <si>
+    <t>"esvento"</t>
+  </si>
+  <si>
+    <t>catarina</t>
+  </si>
+  <si>
+    <t>Concept artist</t>
+  </si>
+  <si>
+    <t>Sophie "Spoot"</t>
   </si>
 </sst>
 </file>
@@ -231,10 +255,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -539,157 +563,177 @@
     </row>
     <row r="2" spans="4:6" ht="30">
       <c r="D2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="4:6">
       <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="4:6">
       <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="4:6">
       <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="4:6">
       <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="4:6">
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="4:6">
       <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="4:6">
       <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="4:6">
       <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="4:6">
       <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="4:6">
       <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="4:6">
       <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="4:6">
       <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="4:6">
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="4:6">
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="4:6">
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="4:6">
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="4:6">
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="4:6">
@@ -758,14 +802,14 @@
       <c r="F33" s="6"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="8">
         <f>COUNTIF(D2:D33,"*")</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 1 new guy
</commit_message>
<xml_diff>
--- a/JumpingJax_bible.xlsx
+++ b/JumpingJax_bible.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\JJ-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235662E2-BB0F-4076-9E68-648B88B8E0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2326FBB-0ED0-4442-B32F-D22C9E591A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Robert Michael Alaniz</t>
+  </si>
+  <si>
+    <t>Daniel Robnik</t>
+  </si>
+  <si>
+    <t>3D modeler</t>
   </si>
 </sst>
 </file>
@@ -273,10 +279,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +564,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -587,15 +593,15 @@
         <v>3</v>
       </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="4:15">
       <c r="D3" s="4" t="s">
@@ -782,8 +788,12 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="4:6">
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="4:6">
@@ -837,14 +847,14 @@
       <c r="F33" s="6"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="8">
         <f>COUNTIF(D2:D33,"*")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added marco to the pack
</commit_message>
<xml_diff>
--- a/JumpingJax_bible.xlsx
+++ b/JumpingJax_bible.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\JJ-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2357D9-3B95-488E-9E35-6174FAAEB6E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E8F50-9BD7-4D68-B487-9B5D0DBE3E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7020" yWindow="2130" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -163,18 +163,31 @@
   </si>
   <si>
     <t>3D modeler</t>
+  </si>
+  <si>
+    <t>Marco Valente</t>
+  </si>
+  <si>
+    <t>Unity gameplay programmer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,12 +270,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -277,12 +290,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,8 +577,8 @@
   </sheetPr>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -797,8 +811,12 @@
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="4:6">
-      <c r="D24" s="4"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="4:6">
@@ -854,7 +872,7 @@
       <c r="C37" s="12"/>
       <c r="D37" s="8">
         <f>COUNTIF(D2:D33,"*")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>